<commit_message>
add estimation of emissions variation through IO methodology (ie, without income rebound effect)
</commit_message>
<xml_diff>
--- a/data_deep/shocks_interventions_large_demand.xlsx
+++ b/data_deep/shocks_interventions_large_demand.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/celia/Documents/These/Production networks/Doc Hubert/toolbox_AEA_vCelia_largecon/data_deep/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/celia/Documents/These/python_projects/production_networks/data_deep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09289BBB-C87C-4041-8D6D-BAC6F48CC215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E27405-E43D-404F-858A-07ECF205C07B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="1540" windowWidth="31560" windowHeight="23480" xr2:uid="{09BEEF32-CDC6-6046-AE7F-58B201249A3A}"/>
+    <workbookView xWindow="2240" yWindow="880" windowWidth="31560" windowHeight="22500" xr2:uid="{09BEEF32-CDC6-6046-AE7F-58B201249A3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -834,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{479E02A8-DACC-FD47-9AA4-9E27891BB81C}">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="I94" sqref="I94"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>